<commit_message>
add text to map
</commit_message>
<xml_diff>
--- a/src/data/nfdimap/participants.xlsx
+++ b/src/data/nfdimap/participants.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68b726b8f38b5cf9/Documents/Git-Repos/nfdimap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68b726b8f38b5cf9/Documents/Git-Repos/nfdi4plants.github.io-1/src/data/nfdimap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="13_ncr:1_{BAB985D0-2B23-2A46-9534-DC236A4373BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D681A6A-8927-41AE-908B-ACBE464514CE}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="13_ncr:1_{BAB985D0-2B23-2A46-9534-DC236A4373BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8320B46D-1FDC-4F04-AF13-A239F641081B}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{067644A4-5F3F-BC4F-88FD-51E3944A351C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{067644A4-5F3F-BC4F-88FD-51E3944A351C}"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Bielefeld University</t>
   </si>
   <si>
-    <t>Senior Advisory Board</t>
-  </si>
-  <si>
     <t>Heterogeneous Information Systems</t>
   </si>
   <si>
@@ -292,12 +289,6 @@
     <t>Ute Krämer</t>
   </si>
   <si>
-    <t>Cristina Martins Rodrigues</t>
-  </si>
-  <si>
-    <t>Project Coordinator</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -469,9 +460,6 @@
     <t>https://www.rz.uni-freiburg.de/rz/organisation/mitarbeiterinnen/schneider</t>
   </si>
   <si>
-    <t>https://www.rz.uni-freiburg.de/rz/organisation/mitarbeiterinnen/martins%20rodrigues</t>
-  </si>
-  <si>
     <t>https://ekvv.uni-bielefeld.de/pers_publ/publ/PersonDetail.jsp?personId=112481313</t>
   </si>
   <si>
@@ -496,9 +484,6 @@
     <t>https://www.helmholtz-muenchen.de/pgsb/forschungseinheit/staff/staff/ma/6373/Prof.%20Dr.-Mayer/index.html</t>
   </si>
   <si>
-    <t>https://www.ceplas.eu/de/forschung/people/dr-dominik-brilhaus/</t>
-  </si>
-  <si>
     <t>https://www.plant-biochemistry.hhu.de/</t>
   </si>
   <si>
@@ -509,6 +494,33 @@
   </si>
   <si>
     <t>https://www.fz-juelich.de/SharedDocs/Kontaktdaten/IBG/IBG-4/DE/Usadel_b_usadel_fz_juelich_de.html?nn=2693740</t>
+  </si>
+  <si>
+    <t>https://www.ceplas.eu/en/research/data-science-and-data-management/</t>
+  </si>
+  <si>
+    <t>Hajira Jabeen</t>
+  </si>
+  <si>
+    <t>Köln</t>
+  </si>
+  <si>
+    <t>Senior Management Board</t>
+  </si>
+  <si>
+    <t>Scientific Advisory Board</t>
+  </si>
+  <si>
+    <t>Data Science and Management</t>
+  </si>
+  <si>
+    <t>Data Science and Management, Botanical Institute</t>
+  </si>
+  <si>
+    <t>University of Cologne</t>
+  </si>
+  <si>
+    <t>https://www.uni-koeln.de/</t>
   </si>
 </sst>
 </file>
@@ -564,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -572,6 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -889,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675F8B27-2A14-6746-AF7B-BBC38C2DA6B4}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -898,8 +911,8 @@
     <col min="1" max="1" width="17.625" style="4" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="4" customWidth="1"/>
     <col min="3" max="4" width="17.625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="83.75" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="48.875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="37.25" style="4" customWidth="1"/>
     <col min="7" max="7" width="17.75" style="4" customWidth="1"/>
     <col min="8" max="8" width="17.875" style="4" customWidth="1"/>
     <col min="9" max="9" width="44.875" style="4" customWidth="1"/>
@@ -910,54 +923,54 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="E2" s="4" t="str">
         <f>"&lt;a href="&amp;B2&amp;C2&amp;B2&amp;"&gt;"&amp;D2&amp;"&lt;/a&gt;"</f>
@@ -967,17 +980,17 @@
         <v>3</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I2" s="4" t="str">
         <f>"&lt;a href="&amp;B2&amp;G2&amp;B2&amp;"&gt;"&amp;H2&amp;"&lt;/a&gt;"</f>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>13</v>
@@ -986,16 +999,16 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="4" t="str">
         <f t="shared" ref="E3:E34" si="0">"&lt;a href="&amp;B3&amp;C3&amp;B3&amp;"&gt;"&amp;D3&amp;"&lt;/a&gt;"</f>
@@ -1005,31 +1018,31 @@
         <v>14</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I3" s="4" t="str">
         <f t="shared" ref="I3:I34" si="1">"&lt;a href="&amp;B3&amp;G3&amp;B3&amp;"&gt;"&amp;H3&amp;"&lt;/a&gt;"</f>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1039,217 +1052,223 @@
         <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I4" s="4" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.ks.uni-freiburg.de/mitarbeiter/klaus_rechert"&gt;Klaus Rechert&lt;/a&gt;</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I5" s="4" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.bio.uni-freiburg.de/ag/reski"&gt;Ralf Reski&lt;/a&gt;</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I6" s="4" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.rz.uni-freiburg.de/rz/organisation/mitarbeiterinnen/schneider"&gt;Gerhard Schneider&lt;/a&gt;</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://www.rz.uni-freiburg.de/rz/organisation/mitarbeiterinnen/martins%20rodrigues"&gt;Cristina Martins Rodrigues&lt;/a&gt;</v>
+        <v>&lt;a href="https://ekvv.uni-bielefeld.de/pers_publ/publ/PersonDetail.jsp?personId=112481313"&gt;Andrea Bräutigam&lt;/a&gt;</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="I8" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
+        <v>&lt;a href="https://uni-bielefeld.de/"&gt;Bielefeld University&lt;/a&gt;</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://ekvv.uni-bielefeld.de/pers_publ/publ/PersonDetail.jsp?personId=112481313"&gt;Andrea Bräutigam&lt;/a&gt;</v>
+        <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/zentrum-fuer-datenverarbeitung/das-zdv/wir-ueber-uns/mitarbeiter/jens-krueger/"&gt;Jens Krüger&lt;/a&gt;</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="I9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="https://uni-bielefeld.de/"&gt;Bielefeld University&lt;/a&gt;</v>
+        <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/zentrum-fuer-datenverarbeitung/das-zdv/wir-ueber-uns/mitarbeiter/jens-krueger/"&gt;Jens Krüger&lt;/a&gt;</v>
+        <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/universitaetsbibliothek/ueber-uns/ansprechpartner/fachreferenten-wissenschaftlicher-dienst/brandt/"&gt;Olaf Brandt&lt;/a&gt;</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>8</v>
@@ -1259,34 +1278,31 @@
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/universitaetsbibliothek/ueber-uns/ansprechpartner/fachreferenten-wissenschaftlicher-dienst/brandt/"&gt;Olaf Brandt&lt;/a&gt;</v>
+        <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/universitaetsbibliothek/ueber-uns/ansprechpartner/fachreferenten-wissenschaftlicher-dienst/doerr/"&gt;Marianne Dörr&lt;/a&gt;</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>8</v>
@@ -1296,7 +1312,7 @@
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1304,23 +1320,23 @@
         <v>51</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/universitaetsbibliothek/ueber-uns/ansprechpartner/fachreferenten-wissenschaftlicher-dienst/doerr/"&gt;Marianne Dörr&lt;/a&gt;</v>
+        <v>&lt;a href="https://uni-tuebingen.de/fakultaeten/mathematisch-naturwissenschaftliche-fakultaet/fachbereiche/zentren/zentrum-fuer-molekularbiologie-der-pflanzen/research/mikrobielle-interaktionen/gruppe/"&gt;Eric Kemen&lt;/a&gt;</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>8</v>
@@ -1330,31 +1346,31 @@
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://uni-tuebingen.de/fakultaeten/mathematisch-naturwissenschaftliche-fakultaet/fachbereiche/zentren/zentrum-fuer-molekularbiologie-der-pflanzen/research/mikrobielle-interaktionen/gruppe/"&gt;Eric Kemen&lt;/a&gt;</v>
+        <v>&lt;a href="https://uni-tuebingen.de/forschung/forschungsinfrastruktur/zentrum-fuer-quantitative-biologie-qbic/team/prof-dr-sven-nahnsen/"&gt;Sven Nahnsen&lt;/a&gt;</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>8</v>
@@ -1364,7 +1380,7 @@
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1372,23 +1388,23 @@
         <v>51</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://uni-tuebingen.de/forschung/forschungsinfrastruktur/zentrum-fuer-quantitative-biologie-qbic/team/prof-dr-sven-nahnsen/"&gt;Sven Nahnsen&lt;/a&gt;</v>
+        <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/zentrum-fuer-datenverarbeitung/das-zdv/wir-ueber-uns/mitarbeiter/prof-dr-thomas-walter/"&gt;Thomas Walter&lt;/a&gt;</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>8</v>
@@ -1398,231 +1414,234 @@
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>82</v>
       </c>
       <c r="E15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/zentrum-fuer-datenverarbeitung/das-zdv/wir-ueber-uns/mitarbeiter/prof-dr-thomas-walter/"&gt;Thomas Walter&lt;/a&gt;</v>
+        <v>&lt;a href="https://www.plant-biochemistry.hhu.de/"&gt;Andreas P. M. Weber&lt;/a&gt;</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="I15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
+        <v>&lt;a href="https://www.hhu.de/"&gt;Heinrich Heine University Düsseldorf&lt;/a&gt;</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://www.ceplas.eu/en/research/data-science-and-data-management/"&gt;Dominik Brillhaus&lt;/a&gt;</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;a href="https://www.hhu.de/"&gt;Heinrich Heine University Düsseldorf&lt;/a&gt;</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://www.plant-biochemistry.hhu.de/"&gt;Andreas P. M. Weber&lt;/a&gt;</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;a href="https://www.hhu.de/"&gt;Heinrich Heine University Düsseldorf&lt;/a&gt;</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="E17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://www.ceplas.eu/en/research/data-science-and-data-management/"&gt;Hajira Jabeen&lt;/a&gt;</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;a href="https://www.uni-koeln.de/"&gt;University of Cologne&lt;/a&gt;</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://www.ceplas.eu/de/forschung/people/dr-dominik-brilhaus/"&gt;Dominik Brillhaus&lt;/a&gt;</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;a href="https://www.hhu.de/"&gt;Heinrich Heine University Düsseldorf&lt;/a&gt;</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="B18" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://www.helmholtz-muenchen.de/pgsb/forschungseinheit/staff/staff/ma/6373/Prof.%20Dr.-Mayer/index.html"&gt;Klaus F. X. Mayer&lt;/a&gt;</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;a href="https://www.helmholtz-muenchen.de/helmholtz-zentrum-muenchen/index.html"&gt;Helmholtz-Zentrum München&lt;/a&gt;</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://www.helmholtz-muenchen.de/pgsb/forschungseinheit/staff/staff/ma/5955/Dr.-Lang/index.html"&gt;Daniel Lang&lt;/a&gt;</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;a href="https://www.helmholtz-muenchen.de/helmholtz-zentrum-muenchen/index.html"&gt;Helmholtz-Zentrum München&lt;/a&gt;</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://rumo.biologie.hu-berlin.de/tbp/index.php/en/people/51-people/head/52-klipp"&gt;Edda Klipp&lt;/a&gt;</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;a href="https://www.hu-berlin.de/de"&gt;Humboldt University Berlin&lt;/a&gt;</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://www.helmholtz-muenchen.de/pgsb/forschungseinheit/staff/staff/ma/6373/Prof.%20Dr.-Mayer/index.html"&gt;Klaus F. X. Mayer&lt;/a&gt;</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;a href="https://www.helmholtz-muenchen.de/helmholtz-zentrum-muenchen/index.html"&gt;Helmholtz-Zentrum München&lt;/a&gt;</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://www.helmholtz-muenchen.de/pgsb/forschungseinheit/staff/staff/ma/5955/Dr.-Lang/index.html"&gt;Daniel Lang&lt;/a&gt;</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;a href="https://www.helmholtz-muenchen.de/helmholtz-zentrum-muenchen/index.html"&gt;Helmholtz-Zentrum München&lt;/a&gt;</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://rumo.biologie.hu-berlin.de/tbp/index.php/en/people/51-people/head/52-klipp"&gt;Edda Klipp&lt;/a&gt;</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;a href="https://www.hu-berlin.de/de"&gt;Humboldt University Berlin&lt;/a&gt;</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1632,7 +1651,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>5</v>
@@ -1642,126 +1661,129 @@
         <v>&lt;a href="https://www.fz-juelich.de/portal/DE/Home/home_node.html"&gt;Jülich Research Center&lt;/a&gt;</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://www.botanik.bio.lmu.de/personen/professuren/leister/"&gt;Dario Leister&lt;/a&gt;</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;a href="https://www.lmu.de/en/"&gt;Ludwigs-Maximilians University Munich&lt;/a&gt;</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://www.mpimp-golm.mpg.de/5224/Alisdair_Fernie"&gt;Alisdair Fernie&lt;/a&gt;</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;a href="https://www.mpimp-golm.mpg.de/"&gt;Max-Planck Institute of Molecular Plant Physiology&lt;/a&gt;</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://www.ruhr-uni-bochum.de/mgpp/Seiten_dt/index_d.html"&gt;Ute Krämer&lt;/a&gt;</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;a href="https://www.ruhr-uni-bochum.de/de"&gt;Ruhr University Bochum&lt;/a&gt;</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://www.botanik.bio.lmu.de/personen/professuren/leister/"&gt;Dario Leister&lt;/a&gt;</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I22" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;a href="https://www.lmu.de/en/"&gt;Ludwigs-Maximilians University Munich&lt;/a&gt;</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://www.mpimp-golm.mpg.de/5224/Alisdair_Fernie"&gt;Alisdair Fernie&lt;/a&gt;</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;a href="https://www.mpimp-golm.mpg.de/"&gt;Max-Planck Institute of Molecular Plant Physiology&lt;/a&gt;</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://www.ruhr-uni-bochum.de/mgpp/Seiten_dt/index_d.html"&gt;Ute Krämer&lt;/a&gt;</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;a href="https://www.ruhr-uni-bochum.de/de"&gt;Ruhr University Bochum&lt;/a&gt;</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="B25" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1771,7 +1793,7 @@
         <v>10</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>11</v>
@@ -1781,34 +1803,34 @@
         <v>&lt;a href="https://www.uni-kl.de/"&gt;Technische Universität Kaiserslautern&lt;/a&gt;</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="http://wwwlgis.informatik.uni-kl.de/cms/his/staff/dessloch/"&gt;Stefan Deßloch&lt;/a&gt;</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>11</v>
@@ -1818,31 +1840,31 @@
         <v>&lt;a href="https://www.uni-kl.de/"&gt;Technische Universität Kaiserslautern&lt;/a&gt;</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://vis.uni-kl.de/team/garth/"&gt;Christoph Garth&lt;/a&gt;</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>11</v>
@@ -1852,34 +1874,34 @@
         <v>&lt;a href="https://www.uni-kl.de/"&gt;Technische Universität Kaiserslautern&lt;/a&gt;</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E28" s="4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://via.cs.uni-kl.de/mitarbeiter/prof-dr-heike-leitte/seite"&gt;Heike Leitte&lt;/a&gt;</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>11</v>
@@ -1889,34 +1911,34 @@
         <v>&lt;a href="https://www.uni-kl.de/"&gt;Technische Universität Kaiserslautern&lt;/a&gt;</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29" s="4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.rhrk.uni-kl.de/wir/organigramm/"&gt;Inga Scheler&lt;/a&gt;</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>11</v>
@@ -1926,123 +1948,123 @@
         <v>&lt;a href="https://www.uni-kl.de/"&gt;Technische Universität Kaiserslautern&lt;/a&gt;</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://evoplant.uni-hohenheim.de/people/schmid/index.html"&gt;Karl Schmid&lt;/a&gt;</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I30" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;a href="https://www.uni-hohenheim.de/"&gt;University of Hohenheim&lt;/a&gt;</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="B31" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://evoplant.uni-hohenheim.de/people/schmid/index.html"&gt;Karl Schmid&lt;/a&gt;</v>
-      </c>
-      <c r="F30" s="4" t="s">
+      <c r="E31" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://phys.uni-hohenheim.de/sandra-schmoeckel"&gt;Sandra Schmöckel&lt;/a&gt;</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I30" s="4" t="str">
+      <c r="G31" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I31" s="4" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-hohenheim.de/"&gt;University of Hohenheim&lt;/a&gt;</v>
       </c>
-      <c r="J30" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://phys.uni-hohenheim.de/sandra-schmoeckel"&gt;Sandra Schmöckel&lt;/a&gt;</v>
-      </c>
-      <c r="F31" s="4" t="s">
+      <c r="J31" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href="https://systembiologie.uni-hohenheim.de/en"&gt;Waltraud Schulze&lt;/a&gt;</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I31" s="4" t="str">
+      <c r="I32" s="4" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-hohenheim.de/"&gt;University of Hohenheim&lt;/a&gt;</v>
       </c>
-      <c r="J31" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;a href="https://systembiologie.uni-hohenheim.de/en"&gt;Waltraud Schulze&lt;/a&gt;</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I32" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;a href="https://www.uni-hohenheim.de/"&gt;University of Hohenheim&lt;/a&gt;</v>
-      </c>
       <c r="J32" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E33" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2052,54 +2074,54 @@
         <v>15</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I33" s="4" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-konstanz.de/"&gt;University of Konstanz&lt;/a&gt;</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E34" s="4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://scikon.uni-konstanz.de/personen/profile/anja.oberlaender/"&gt;Anja Oberländer&lt;/a&gt;</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I34" s="4" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-konstanz.de/"&gt;University of Konstanz&lt;/a&gt;</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2120,17 +2142,19 @@
     <hyperlink ref="G31" r:id="rId1" xr:uid="{9F912C88-2558-4F38-B74B-A756697FD20B}"/>
     <hyperlink ref="G32" r:id="rId2" xr:uid="{0647AE71-4486-4344-90B8-D320623185F4}"/>
     <hyperlink ref="G30" r:id="rId3" xr:uid="{8593821B-C05A-4D34-B0DF-9C1DD7395467}"/>
+    <hyperlink ref="C17" r:id="rId4" xr:uid="{FC4D73A5-FC29-40A2-8C46-340A50A6DC4B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCF9441-CE5A-BB4B-81C4-F29D4A249B72}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2143,15 +2167,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2">
         <v>47.994132999999998</v>
@@ -2162,7 +2186,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2">
         <v>52.036842999999998</v>
@@ -2173,7 +2197,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2">
         <v>48.530724999999997</v>
@@ -2184,7 +2208,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B5" s="2">
         <v>51.191947999999996</v>
@@ -2195,7 +2219,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B6" s="2">
         <v>48.385803000000003</v>
@@ -2206,7 +2230,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B7" s="2">
         <v>52.520156</v>
@@ -2217,7 +2241,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B8" s="2">
         <v>50.906416999999998</v>
@@ -2228,7 +2252,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B9" s="2">
         <v>52.416276000000003</v>
@@ -2239,7 +2263,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B10" s="2">
         <v>51.445622999999998</v>
@@ -2250,7 +2274,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B11" s="2">
         <v>49.426779000000003</v>
@@ -2261,7 +2285,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B12" s="2">
         <v>48.713600999999997</v>
@@ -2272,7 +2296,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B13" s="2">
         <v>47.690018000000002</v>
@@ -2283,13 +2307,24 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B14" s="2">
         <v>50.921489999999999</v>
       </c>
       <c r="C14" s="2">
         <v>6.3626699999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="2">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="C15" s="2">
+        <v>6.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change datahub info text
</commit_message>
<xml_diff>
--- a/src/data/nfdimap/participants.xlsx
+++ b/src/data/nfdimap/participants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68b726b8f38b5cf9/Documents/Git-Repos/nfdi4plants.github.io/src/data/nfdimap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Documents\Git-Repos\nfdi4plants.github.io-1\src\data\nfdimap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{BAB985D0-2B23-2A46-9534-DC236A4373BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27ADBA4B-4A7A-4656-9630-65633B26C8BD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54A5FDF-D95A-4637-A59F-B615A6421743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="4905" windowWidth="29040" windowHeight="17640" xr2:uid="{067644A4-5F3F-BC4F-88FD-51E3944A351C}"/>
+    <workbookView xWindow="-28920" yWindow="5310" windowWidth="29040" windowHeight="17520" xr2:uid="{067644A4-5F3F-BC4F-88FD-51E3944A351C}"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -521,6 +521,99 @@
   </si>
   <si>
     <t>Dominik Brilhaus</t>
+  </si>
+  <si>
+    <t>Kehl</t>
+  </si>
+  <si>
+    <t>Golm</t>
+  </si>
+  <si>
+    <t>Neustadt Wstr.</t>
+  </si>
+  <si>
+    <t>Hannover</t>
+  </si>
+  <si>
+    <t>Marburg</t>
+  </si>
+  <si>
+    <t>Freising</t>
+  </si>
+  <si>
+    <t>Regensburg</t>
+  </si>
+  <si>
+    <t>Halle (Saale)</t>
+  </si>
+  <si>
+    <t>Base4NFDI - IAM4nfdi</t>
+  </si>
+  <si>
+    <t>Base4NFDI - PID4NFDI</t>
+  </si>
+  <si>
+    <t>Base4NFDI - RDMTraining4All</t>
+  </si>
+  <si>
+    <t>Base4NFDI - TS4nfdi</t>
+  </si>
+  <si>
+    <t>Base4NFDI - nfdi.software</t>
+  </si>
+  <si>
+    <t>DiP-KS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datenkompetenzzentrum - LAB_DaiTA </t>
+  </si>
+  <si>
+    <t>Datenkompetenzzentrum - de.KCD</t>
+  </si>
+  <si>
+    <t>Datenkompetenzzentrum - LSData.NET</t>
+  </si>
+  <si>
+    <t>TRR 356: PlantMicrobe</t>
+  </si>
+  <si>
+    <t>SFB 1664</t>
+  </si>
+  <si>
+    <t>SFB 1597: Small Data</t>
+  </si>
+  <si>
+    <t>EXC: HighQ</t>
+  </si>
+  <si>
+    <t>Highly sensitive bioluminescence and fluorescence imaging system for large fields of view</t>
+  </si>
+  <si>
+    <t>NFDI - METHODS</t>
+  </si>
+  <si>
+    <t>SPP 2237: MAdLand</t>
+  </si>
+  <si>
+    <t>Linking organelles by actin tracks to establish membrane contact sites</t>
+  </si>
+  <si>
+    <t>In-depth characterisation of novel components involved in transgene silencing and a(biotic) stress defense</t>
+  </si>
+  <si>
+    <t>FOR 5235: CSCS</t>
+  </si>
+  <si>
+    <t>FOR 3000</t>
+  </si>
+  <si>
+    <t>AutoPlanDat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freiburg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halle (Saale) </t>
   </si>
 </sst>
 </file>
@@ -530,7 +623,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -550,6 +643,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -580,12 +680,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -901,1250 +1001,1409 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675F8B27-2A14-6746-AF7B-BBC38C2DA6B4}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="17.625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="7.625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="17.625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="48.875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="37.25" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.75" style="4" customWidth="1"/>
-    <col min="8" max="8" width="47.125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="44.875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.375" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="4"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="4" width="17.625" customWidth="1"/>
+    <col min="5" max="5" width="48.875" customWidth="1"/>
+    <col min="6" max="6" width="37.25" customWidth="1"/>
+    <col min="7" max="7" width="17.75" customWidth="1"/>
+    <col min="8" max="8" width="47.125" customWidth="1"/>
+    <col min="9" max="9" width="44.875" customWidth="1"/>
+    <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="4" t="str">
+      <c r="E2" t="str">
         <f>"&lt;a href="&amp;B2&amp;C2&amp;B2&amp;"&gt;"&amp;D2&amp;"&lt;/a&gt;"</f>
         <v>&lt;a href="https://www.ks.uni-freiburg.de/mitarbeiter/Dirk_von_Suchodoletz"&gt;Dirk von Suchodoletz&lt;/a&gt;</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>108</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>109</v>
       </c>
-      <c r="I2" s="4" t="str">
+      <c r="I2" t="str">
         <f>"&lt;a href="&amp;B2&amp;G2&amp;B2&amp;"&gt;"&amp;H2&amp;"&lt;/a&gt;"</f>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="5"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="4" t="str">
+      <c r="E3" t="str">
         <f t="shared" ref="E3:E34" si="0">"&lt;a href="&amp;B3&amp;C3&amp;B3&amp;"&gt;"&amp;D3&amp;"&lt;/a&gt;"</f>
         <v>&lt;a href="http://www.bioinf.uni-freiburg.de/~backofen/"&gt;Rolf Backofen&lt;/a&gt;</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="4" t="str">
+      <c r="I3" t="str">
         <f t="shared" ref="I3:I34" si="1">"&lt;a href="&amp;B3&amp;G3&amp;B3&amp;"&gt;"&amp;H3&amp;"&lt;/a&gt;"</f>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="4" t="str">
+      <c r="E4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.experten.uni-freiburg.de/pr/experts/bjoern-gruening"&gt;Björn Grüning&lt;/a&gt;</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="4" t="str">
+      <c r="I4" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="4" t="str">
+      <c r="E5" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.ks.uni-freiburg.de/mitarbeiter/klaus_rechert"&gt;Klaus Rechert&lt;/a&gt;</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="4" t="str">
+      <c r="I5" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="4" t="str">
+      <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.bio.uni-freiburg.de/ag/reski"&gt;Ralf Reski&lt;/a&gt;</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="4" t="str">
+      <c r="I6" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" t="s">
         <v>87</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="4" t="str">
+      <c r="E7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.rz.uni-freiburg.de/rz/organisation/mitarbeiterinnen/schneider"&gt;Gerhard Schneider&lt;/a&gt;</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" t="s">
         <v>108</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="4" t="str">
+      <c r="I7" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-freiburg.de/"&gt;Albrecht-Ludwigs University of Freiburg&lt;/a&gt;</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="4" t="str">
+      <c r="E8" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://ekvv.uni-bielefeld.de/pers_publ/publ/PersonDetail.jsp?personId=112481313"&gt;Andrea Bräutigam&lt;/a&gt;</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" t="s">
         <v>110</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="4" t="str">
+      <c r="I8" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-bielefeld.de/"&gt;Bielefeld University&lt;/a&gt;</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="4" t="str">
+      <c r="E9" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/zentrum-fuer-datenverarbeitung/das-zdv/wir-ueber-uns/mitarbeiter/jens-krueger/"&gt;Jens Krüger&lt;/a&gt;</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" t="s">
         <v>111</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="4" t="str">
+      <c r="I9" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" t="s">
         <v>89</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" t="s">
         <v>142</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="4" t="str">
+      <c r="E10" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/universitaetsbibliothek/ueber-uns/ansprechpartner/fachreferenten-wissenschaftlicher-dienst/brandt/"&gt;Olaf Brandt&lt;/a&gt;</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" t="s">
         <v>111</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="4" t="str">
+      <c r="I10" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="4" t="str">
+      <c r="E11" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/universitaetsbibliothek/ueber-uns/ansprechpartner/fachreferenten-wissenschaftlicher-dienst/doerr/"&gt;Marianne Dörr&lt;/a&gt;</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" t="s">
         <v>111</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="4" t="str">
+      <c r="I11" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="4" t="str">
+      <c r="E12" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://uni-tuebingen.de/fakultaeten/mathematisch-naturwissenschaftliche-fakultaet/fachbereiche/zentren/zentrum-fuer-molekularbiologie-der-pflanzen/research/mikrobielle-interaktionen/gruppe/"&gt;Eric Kemen&lt;/a&gt;</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="4" t="str">
+      <c r="I12" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A13" s="4" t="s">
+      <c r="A13" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" t="s">
         <v>150</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="4" t="str">
+      <c r="E13" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://uni-tuebingen.de/forschung/forschungsinfrastruktur/zentrum-fuer-quantitative-biologie-qbic/team/prof-dr-sven-nahnsen/"&gt;Sven Nahnsen&lt;/a&gt;</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" t="s">
         <v>111</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="4" t="str">
+      <c r="I13" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A14" s="4" t="s">
+      <c r="A14" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="8" t="str">
+      <c r="E14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://uni-tuebingen.de/einrichtungen/zentrum-fuer-datenverarbeitung/das-zdv/wir-ueber-uns/mitarbeiter/prof-dr-thomas-walter/"&gt;Thomas Walter&lt;/a&gt;</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="4" t="str">
+      <c r="I14" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://uni-tuebingen.de/"&gt;Eberhard Karls University Tübingen&lt;/a&gt;</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A15" s="4" t="s">
+      <c r="A15" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="8" t="str">
+      <c r="E15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.plant-biochemistry.hhu.de/"&gt;Andreas P. M. Weber&lt;/a&gt;</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="4" t="str">
+      <c r="I15" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.hhu.de/"&gt;Heinrich Heine University Düsseldorf&lt;/a&gt;</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" t="s">
         <v>98</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A16" s="4" t="s">
+      <c r="A16" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E16" s="8" t="str">
+      <c r="E16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.ceplas.eu/en/research/data-science-and-data-management/"&gt;Dominik Brilhaus&lt;/a&gt;</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="4" t="str">
+      <c r="I16" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.hhu.de/"&gt;Heinrich Heine University Düsseldorf&lt;/a&gt;</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" t="s">
         <v>98</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A17" s="4" t="s">
+      <c r="A17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E17" s="8" t="str">
+      <c r="E17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.ceplas.eu/en/research/data-science-and-data-management/"&gt;Hajira Jabeen&lt;/a&gt;</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" t="s">
         <v>159</v>
       </c>
-      <c r="I17" s="4" t="str">
+      <c r="I17" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-koeln.de/"&gt;University of Cologne&lt;/a&gt;</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" t="s">
         <v>154</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A18" s="4" t="s">
+      <c r="A18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="8" t="str">
+      <c r="E18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.helmholtz-muenchen.de/pgsb/forschungseinheit/staff/staff/ma/6373/Prof.%20Dr.-Mayer/index.html"&gt;Klaus F. X. Mayer&lt;/a&gt;</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="4" t="str">
+      <c r="I18" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.helmholtz-muenchen.de/helmholtz-zentrum-muenchen/index.html"&gt;Helmholtz-Zentrum München&lt;/a&gt;</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A19" s="4" t="s">
+      <c r="A19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="8" t="str">
+      <c r="E19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.helmholtz-muenchen.de/pgsb/forschungseinheit/staff/staff/ma/5955/Dr.-Lang/index.html"&gt;Daniel Lang&lt;/a&gt;</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="4" t="str">
+      <c r="I19" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.helmholtz-muenchen.de/helmholtz-zentrum-muenchen/index.html"&gt;Helmholtz-Zentrum München&lt;/a&gt;</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A20" s="4" t="s">
+      <c r="A20" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="8" t="str">
+      <c r="E20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://rumo.biologie.hu-berlin.de/tbp/index.php/en/people/51-people/head/52-klipp"&gt;Edda Klipp&lt;/a&gt;</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="4" t="str">
+      <c r="I20" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.hu-berlin.de/de"&gt;Humboldt University Berlin&lt;/a&gt;</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A21" s="4" t="s">
+      <c r="A21" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="8" t="str">
+      <c r="E21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.fz-juelich.de/SharedDocs/Kontaktdaten/IBG/IBG-4/DE/Usadel_b_usadel_fz_juelich_de.html?nn=2693740"&gt;Björn Usadel&lt;/a&gt;</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="4" t="str">
+      <c r="I21" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.fz-juelich.de/portal/DE/Home/home_node.html"&gt;Jülich Research Center&lt;/a&gt;</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" t="s">
         <v>88</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A22" s="4" t="s">
+      <c r="A22" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="8" t="str">
+      <c r="E22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.botanik.bio.lmu.de/personen/professuren/leister/"&gt;Dario Leister&lt;/a&gt;</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="4" t="str">
+      <c r="I22" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.lmu.de/en/"&gt;Ludwigs-Maximilians University Munich&lt;/a&gt;</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A23" s="4" t="s">
+      <c r="A23" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="8" t="s">
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="8" t="str">
+      <c r="E23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.mpimp-golm.mpg.de/5224/Alisdair_Fernie"&gt;Alisdair Fernie&lt;/a&gt;</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" t="s">
         <v>20</v>
       </c>
-      <c r="I23" s="4" t="str">
+      <c r="I23" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.mpimp-golm.mpg.de/"&gt;Max-Planck Institute of Molecular Plant Physiology&lt;/a&gt;</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A24" s="4" t="s">
+      <c r="A24" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="B24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="8" t="str">
+      <c r="E24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.ruhr-uni-bochum.de/mgpp/Seiten_dt/index_d.html"&gt;Ute Krämer&lt;/a&gt;</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" t="s">
         <v>27</v>
       </c>
-      <c r="I24" s="4" t="str">
+      <c r="I24" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.ruhr-uni-bochum.de/de"&gt;Ruhr University Bochum&lt;/a&gt;</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" t="s">
         <v>95</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A25" s="4" t="s">
+      <c r="A25" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="B25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="8" t="str">
+      <c r="E25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.bio.uni-kl.de/organisation/mitarbeiter/m-o/muehlhaus-timo"&gt;Timo Mühlhaus&lt;/a&gt;</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="4" t="str">
+      <c r="I25" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-kl.de/"&gt;Technische Universität Kaiserslautern&lt;/a&gt;</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" t="s">
         <v>90</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A26" s="4" t="s">
+      <c r="A26" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="8" t="s">
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="8" t="str">
+      <c r="E26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="http://wwwlgis.informatik.uni-kl.de/cms/his/staff/dessloch/"&gt;Stefan Deßloch&lt;/a&gt;</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" t="s">
         <v>11</v>
       </c>
-      <c r="I26" s="4" t="str">
+      <c r="I26" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-kl.de/"&gt;Technische Universität Kaiserslautern&lt;/a&gt;</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A27" s="4" t="s">
+      <c r="A27" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="B27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="8" t="str">
+      <c r="E27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://vis.uni-kl.de/team/garth/"&gt;Christoph Garth&lt;/a&gt;</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" t="s">
         <v>11</v>
       </c>
-      <c r="I27" s="4" t="str">
+      <c r="I27" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-kl.de/"&gt;Technische Universität Kaiserslautern&lt;/a&gt;</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" t="s">
         <v>90</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A28" s="4" t="s">
+      <c r="A28" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="8" t="s">
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="8" t="str">
+      <c r="E28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://via.cs.uni-kl.de/mitarbeiter/prof-dr-heike-leitte/seite"&gt;Heike Leitte&lt;/a&gt;</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="4" t="str">
+      <c r="I28" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-kl.de/"&gt;Technische Universität Kaiserslautern&lt;/a&gt;</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J28" t="s">
         <v>90</v>
       </c>
-      <c r="K28" s="7" t="s">
+      <c r="K28" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A29" s="4" t="s">
+      <c r="A29" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C29" s="8" t="s">
+      <c r="B29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E29" s="8" t="str">
+      <c r="E29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://www.rhrk.uni-kl.de/wir/organigramm/"&gt;Inga Scheler&lt;/a&gt;</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="4" t="str">
+      <c r="I29" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-kl.de/"&gt;Technische Universität Kaiserslautern&lt;/a&gt;</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A30" s="4" t="s">
+      <c r="A30" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="B30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="8" t="str">
+      <c r="E30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://evoplant.uni-hohenheim.de/people/schmid/index.html"&gt;Karl Schmid&lt;/a&gt;</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G30" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" t="s">
         <v>41</v>
       </c>
-      <c r="I30" s="4" t="str">
+      <c r="I30" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-hohenheim.de/"&gt;University of Hohenheim&lt;/a&gt;</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A31" s="4" t="s">
+      <c r="A31" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="8" t="s">
+      <c r="B31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="8" t="str">
+      <c r="E31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://phys.uni-hohenheim.de/sandra-schmoeckel"&gt;Sandra Schmöckel&lt;/a&gt;</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" t="s">
         <v>41</v>
       </c>
-      <c r="I31" s="4" t="str">
+      <c r="I31" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-hohenheim.de/"&gt;University of Hohenheim&lt;/a&gt;</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A32" s="4" t="s">
+      <c r="A32" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="8" t="s">
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="8" t="str">
+      <c r="E32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://systembiologie.uni-hohenheim.de/en"&gt;Waltraud Schulze&lt;/a&gt;</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H32" t="s">
         <v>41</v>
       </c>
-      <c r="I32" s="4" t="str">
+      <c r="I32" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-hohenheim.de/"&gt;University of Hohenheim&lt;/a&gt;</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J32" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A33" s="4" t="s">
+      <c r="A33" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="8" t="s">
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E33" s="8" t="str">
+      <c r="E33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://scikon.uni-konstanz.de/personen/profile/petra.haetscher/"&gt;Petra Hätscher&lt;/a&gt;</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H33" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="4" t="str">
+      <c r="I33" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-konstanz.de/"&gt;University of Konstanz&lt;/a&gt;</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J33" t="s">
         <v>93</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K33" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A34" s="4" t="s">
+      <c r="A34" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="8" t="s">
+      <c r="B34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E34" s="8" t="str">
+      <c r="E34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;a href="https://scikon.uni-konstanz.de/personen/profile/anja.oberlaender/"&gt;Anja Oberländer&lt;/a&gt;</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H34" t="s">
         <v>22</v>
       </c>
-      <c r="I34" s="4" t="str">
+      <c r="I34" t="str">
         <f t="shared" si="1"/>
         <v>&lt;a href="https://www.uni-konstanz.de/"&gt;University of Konstanz&lt;/a&gt;</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="J34" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
+      <c r="D35" t="s">
+        <v>170</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="J35" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="D36" t="s">
+        <v>171</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="J36" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="D37" t="s">
+        <v>172</v>
+      </c>
+      <c r="J37" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D38" t="s">
+        <v>173</v>
+      </c>
+      <c r="J38" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D39" t="s">
+        <v>174</v>
+      </c>
+      <c r="J39" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D40" t="s">
+        <v>175</v>
+      </c>
+      <c r="J40" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D41" t="s">
+        <v>176</v>
+      </c>
+      <c r="J41" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D42" t="s">
+        <v>177</v>
+      </c>
+      <c r="J42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D43" t="s">
+        <v>178</v>
+      </c>
+      <c r="J43" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D44" t="s">
+        <v>179</v>
+      </c>
+      <c r="J44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D45" t="s">
+        <v>180</v>
+      </c>
+      <c r="J45" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D46" t="s">
+        <v>181</v>
+      </c>
+      <c r="J46" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D47" t="s">
+        <v>182</v>
+      </c>
+      <c r="J47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D48" t="s">
+        <v>183</v>
+      </c>
+      <c r="J48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.5">
+      <c r="D49" t="s">
+        <v>184</v>
+      </c>
+      <c r="J49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.5">
+      <c r="D50" t="s">
+        <v>185</v>
+      </c>
+      <c r="J50" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.5">
+      <c r="D51" t="s">
+        <v>186</v>
+      </c>
+      <c r="J51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="4:10" x14ac:dyDescent="0.5">
+      <c r="D52" t="s">
+        <v>187</v>
+      </c>
+      <c r="J52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="4:10" x14ac:dyDescent="0.5">
+      <c r="D53" t="s">
+        <v>188</v>
+      </c>
+      <c r="J53" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="4:10" x14ac:dyDescent="0.5">
+      <c r="D54" t="s">
+        <v>189</v>
+      </c>
+      <c r="J54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="4:10" x14ac:dyDescent="0.5">
+      <c r="D55" t="s">
+        <v>190</v>
+      </c>
+      <c r="H55" t="s">
+        <v>22</v>
+      </c>
+      <c r="J55" t="s">
+        <v>165</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L38">
-    <sortCondition ref="H2:H38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L37">
+    <sortCondition ref="H2:H37"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="G31" r:id="rId1" xr:uid="{9F912C88-2558-4F38-B74B-A756697FD20B}"/>
@@ -2159,10 +2418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCF9441-CE5A-BB4B-81C4-F29D4A249B72}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2248,13 +2507,13 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
+      <c r="A8" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="8">
         <v>50.906416999999998</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="8">
         <v>6.4046719999999997</v>
       </c>
     </row>
@@ -2333,6 +2592,94 @@
       </c>
       <c r="C15" s="2">
         <v>6.9602785999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="2">
+        <v>48.572969999999998</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7.8152299999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="2">
+        <v>52.4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>12.966699999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" s="2">
+        <v>49.340510000000002</v>
+      </c>
+      <c r="C18" s="2">
+        <v>8.1331500000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="2">
+        <v>52.373919999999998</v>
+      </c>
+      <c r="C19" s="2">
+        <v>9.7356029999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" s="2">
+        <v>51.482799999999997</v>
+      </c>
+      <c r="C20" s="2">
+        <v>11.639200000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B21" s="2">
+        <v>50.809040000000003</v>
+      </c>
+      <c r="C21" s="2">
+        <v>8.7706900000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="2">
+        <v>48.403509999999997</v>
+      </c>
+      <c r="C22" s="2">
+        <v>11.748760000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="2">
+        <v>49.0167</v>
+      </c>
+      <c r="C23" s="2">
+        <v>12.083299999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test bug fix again
</commit_message>
<xml_diff>
--- a/src/data/nfdimap/participants.xlsx
+++ b/src/data/nfdimap/participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nfdi4plant-my.sharepoint.com/personal/cmrodrigues_nfdi4plants_org/Documents/cmrodrigues/7_Zwischenspeicher/Test Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{CCE9C233-1E9E-41AD-884D-99AF607F5230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{930D1A51-C807-485F-880C-4A24BA6C7967}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{CCE9C233-1E9E-41AD-884D-99AF607F5230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9082548-2010-4748-A210-721511EA6730}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{067644A4-5F3F-BC4F-88FD-51E3944A351C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{067644A4-5F3F-BC4F-88FD-51E3944A351C}"/>
   </bookViews>
   <sheets>
     <sheet name="People" sheetId="1" r:id="rId1"/>
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675F8B27-2A14-6746-AF7B-BBC38C2DA6B4}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1052,11 +1052,11 @@
     <col min="1" max="1" width="17.625" customWidth="1"/>
     <col min="2" max="2" width="7.625" customWidth="1"/>
     <col min="3" max="4" width="17.625" customWidth="1"/>
-    <col min="5" max="5" width="48.875" customWidth="1"/>
+    <col min="5" max="5" width="215.0625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.25" customWidth="1"/>
     <col min="7" max="7" width="17.75" customWidth="1"/>
     <col min="8" max="8" width="47.125" customWidth="1"/>
-    <col min="9" max="9" width="44.875" customWidth="1"/>
+    <col min="9" max="9" width="119.4375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.375" customWidth="1"/>
   </cols>
@@ -2693,8 +2693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCF9441-CE5A-BB4B-81C4-F29D4A249B72}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>